<commit_message>
1) Fixing the pinout on the PPS330D to match what is on the DEB429A -- the select lines are still off though. 2) Updating the BOM for the PLR5010D -- adding the base resistor for the BJTs
</commit_message>
<xml_diff>
--- a/Hardware/LAB-PLR5010D/docs/LAB-PLR5010D-Rev1BOM.xlsx
+++ b/Hardware/LAB-PLR5010D/docs/LAB-PLR5010D-Rev1BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15810" yWindow="-30" windowWidth="18345" windowHeight="13440"/>
+    <workbookView xWindow="20670" yWindow="-30" windowWidth="18345" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>BILL OF MATERIALS</t>
   </si>
@@ -193,13 +193,25 @@
   </si>
   <si>
     <t>Total Board Cost:</t>
+  </si>
+  <si>
+    <t>R1, R2</t>
+  </si>
+  <si>
+    <t>RC1608F391CS</t>
+  </si>
+  <si>
+    <t>RES SMD 390 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>1276-4610-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +271,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -389,7 +407,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -462,6 +480,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -483,8 +503,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -792,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,11 +842,11 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2"/>
       <c r="F2" s="8"/>
       <c r="G2" s="2"/>
@@ -838,10 +857,10 @@
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="32"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="2"/>
       <c r="F3" s="8"/>
       <c r="G3" s="2"/>
@@ -852,10 +871,10 @@
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="2"/>
       <c r="F4" s="8"/>
       <c r="G4" s="2"/>
@@ -866,10 +885,10 @@
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="32"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="2"/>
       <c r="F5" s="8"/>
       <c r="G5" s="2"/>
@@ -880,10 +899,10 @@
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="2"/>
       <c r="F6" s="8"/>
       <c r="G6" s="2"/>
@@ -1000,7 +1019,7 @@
         <v>0.2059</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10:L26" si="0">K10*G10</f>
+        <f t="shared" ref="L10:L16" si="0">K10*G10</f>
         <v>0.4118</v>
       </c>
     </row>
@@ -1032,7 +1051,7 @@
       <c r="J11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="35">
+      <c r="K11" s="28">
         <v>6.9173999999999998</v>
       </c>
       <c r="L11">
@@ -1069,7 +1088,7 @@
       <c r="J12" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="35">
+      <c r="K12" s="28">
         <v>0.66359999999999997</v>
       </c>
       <c r="L12">
@@ -1105,7 +1124,7 @@
       <c r="J13" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="35">
+      <c r="K13" s="28">
         <v>3.5060000000000001E-2</v>
       </c>
       <c r="L13">
@@ -1141,7 +1160,7 @@
       <c r="J14" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="35">
+      <c r="K14" s="28">
         <v>4.2599999999999999E-3</v>
       </c>
       <c r="L14">
@@ -1177,7 +1196,7 @@
       <c r="J15" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="K15" s="35">
+      <c r="K15" s="28">
         <v>7.7999999999999996E-3</v>
       </c>
       <c r="L15">
@@ -1186,111 +1205,138 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="14"/>
-      <c r="K16" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="L16" s="36">
-        <f>SUM(L9:L15)</f>
-        <v>9.4532199999999982</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>8</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="14">
+        <v>2</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K16" s="28">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>1.14E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="16"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="15"/>
       <c r="G17" s="14"/>
-      <c r="K17" s="35"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="L17" s="29">
+        <f>SUM(L9:L16)</f>
+        <v>9.4646199999999983</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="15"/>
       <c r="G18" s="14"/>
-      <c r="K18" s="35"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="28"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="16"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="15"/>
       <c r="G19" s="14"/>
-      <c r="K19" s="35"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="28"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="16"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="15"/>
       <c r="G20" s="14"/>
-      <c r="K20" s="35"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="28"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="15"/>
       <c r="G21" s="14"/>
-      <c r="K21" s="35"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="28"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="16"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="15"/>
       <c r="G22" s="14"/>
-      <c r="K22" s="35"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="28"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="16"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="15"/>
       <c r="G23" s="14"/>
-      <c r="K23" s="35"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="28"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="16"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="15"/>
       <c r="G24" s="14"/>
-      <c r="K24" s="35"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="28"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="16"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="15"/>
       <c r="G25" s="14"/>
-      <c r="K25" s="35"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="28"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="16"/>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="15"/>
       <c r="G26" s="14"/>
-      <c r="K26" s="35"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="28"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="16"/>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
@@ -1298,7 +1344,7 @@
       <c r="F27" s="15"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
       <c r="D28" s="14"/>
@@ -1306,7 +1352,7 @@
       <c r="F28" s="15"/>
       <c r="G28" s="14"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="16"/>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
@@ -1314,7 +1360,7 @@
       <c r="F29" s="15"/>
       <c r="G29" s="14"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="16"/>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
@@ -1322,7 +1368,7 @@
       <c r="F30" s="15"/>
       <c r="G30" s="14"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="16"/>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
@@ -1330,7 +1376,7 @@
       <c r="F31" s="15"/>
       <c r="G31" s="14"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="16"/>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
@@ -1468,8 +1514,10 @@
     <hyperlink ref="J10" r:id="rId8"/>
     <hyperlink ref="B15" r:id="rId9" display="http://www.digikey.com/product-detail/en/CL10B103MB8NCNC/1276-1927-1-ND/3890013"/>
     <hyperlink ref="J15" r:id="rId10" display="http://www.digikey.com/product-detail/en/CL10B103MB8NCNC/1276-1927-1-ND/3890013"/>
+    <hyperlink ref="B16" r:id="rId11" display="http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/RC1608F391CS/1276-4610-1-ND/3967582"/>
+    <hyperlink ref="J16" r:id="rId12" display="http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/RC1608F391CS/1276-4610-1-ND/3967582"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId11"/>
+  <pageSetup paperSize="9" scale="50" orientation="landscape" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>